<commit_message>
changing buckets code and rebalancing na scheduling
</commit_message>
<xml_diff>
--- a/schedules.xlsx
+++ b/schedules.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="70">
   <si>
     <t>orderID</t>
   </si>
@@ -45,172 +45,187 @@
     <t>Scheduled Machine</t>
   </si>
   <si>
-    <t>698326</t>
-  </si>
-  <si>
-    <t>0698679-C</t>
-  </si>
-  <si>
-    <t>0697795-C</t>
-  </si>
-  <si>
-    <t>698000</t>
-  </si>
-  <si>
-    <t>0698477-C</t>
-  </si>
-  <si>
-    <t>0697952-C</t>
-  </si>
-  <si>
-    <t>697951</t>
-  </si>
-  <si>
-    <t>B090-350-09</t>
-  </si>
-  <si>
-    <t>B090-466-09</t>
-  </si>
-  <si>
-    <t>B090-813-61</t>
-  </si>
-  <si>
-    <t>54</t>
+    <t>697612</t>
+  </si>
+  <si>
+    <t>697124</t>
+  </si>
+  <si>
+    <t>697125</t>
+  </si>
+  <si>
+    <t>0696823-C</t>
+  </si>
+  <si>
+    <t>697927</t>
+  </si>
+  <si>
+    <t>0696949-C</t>
+  </si>
+  <si>
+    <t>0696782-C</t>
+  </si>
+  <si>
+    <t>B670-813-49</t>
+  </si>
+  <si>
+    <t>B672-813-49</t>
+  </si>
+  <si>
+    <t>C193-602-70</t>
   </si>
   <si>
     <t>na</t>
   </si>
   <si>
-    <t>2022-04-11 00:00:00</t>
-  </si>
-  <si>
-    <t>2022-04-18 00:00:00</t>
+    <t>2022-03-22 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-03-25 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-03-29 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-03-30 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>0696893-C</t>
+  </si>
+  <si>
+    <t>697005</t>
+  </si>
+  <si>
+    <t>0697360-C</t>
+  </si>
+  <si>
+    <t>0697006-C</t>
+  </si>
+  <si>
+    <t>0697925-C</t>
+  </si>
+  <si>
+    <t>0697923-C</t>
+  </si>
+  <si>
+    <t>0697922-C</t>
+  </si>
+  <si>
+    <t>697921</t>
+  </si>
+  <si>
+    <t>696720</t>
+  </si>
+  <si>
+    <t>0696740-C</t>
+  </si>
+  <si>
+    <t>698221</t>
+  </si>
+  <si>
+    <t>697611</t>
+  </si>
+  <si>
+    <t>697510</t>
+  </si>
+  <si>
+    <t>697513</t>
+  </si>
+  <si>
+    <t>697505</t>
+  </si>
+  <si>
+    <t>697603</t>
+  </si>
+  <si>
+    <t>697604</t>
+  </si>
+  <si>
+    <t>698087</t>
+  </si>
+  <si>
+    <t>697715</t>
+  </si>
+  <si>
+    <t>698056</t>
+  </si>
+  <si>
+    <t>0698057-C</t>
+  </si>
+  <si>
+    <t>697494</t>
+  </si>
+  <si>
+    <t>0697495-C</t>
+  </si>
+  <si>
+    <t>697727</t>
+  </si>
+  <si>
+    <t>697509</t>
+  </si>
+  <si>
+    <t>697711</t>
+  </si>
+  <si>
+    <t>697710</t>
+  </si>
+  <si>
+    <t>697708</t>
+  </si>
+  <si>
+    <t>697725</t>
+  </si>
+  <si>
+    <t>697726</t>
+  </si>
+  <si>
+    <t>697723</t>
+  </si>
+  <si>
+    <t>697722</t>
+  </si>
+  <si>
+    <t>697720</t>
+  </si>
+  <si>
+    <t>697719</t>
+  </si>
+  <si>
+    <t>697514</t>
+  </si>
+  <si>
+    <t>0697724-C</t>
+  </si>
+  <si>
+    <t>697721</t>
+  </si>
+  <si>
+    <t>7555-617-70</t>
+  </si>
+  <si>
+    <t>55</t>
   </si>
   <si>
     <t>2022-04-04 00:00:00</t>
   </si>
   <si>
-    <t>2022-04-21 00:00:00</t>
-  </si>
-  <si>
-    <t>698857</t>
-  </si>
-  <si>
-    <t>0696893-C</t>
-  </si>
-  <si>
-    <t>0697994-C-S</t>
-  </si>
-  <si>
-    <t>0698470-C</t>
-  </si>
-  <si>
-    <t>0698280-C</t>
-  </si>
-  <si>
-    <t>698282</t>
-  </si>
-  <si>
-    <t>697970</t>
-  </si>
-  <si>
-    <t>698705</t>
-  </si>
-  <si>
-    <t>0697964-C</t>
-  </si>
-  <si>
-    <t>698946</t>
-  </si>
-  <si>
-    <t>697962</t>
-  </si>
-  <si>
-    <t>0697949-C</t>
-  </si>
-  <si>
-    <t>0698657-C</t>
-  </si>
-  <si>
-    <t>0698896-C</t>
-  </si>
-  <si>
-    <t>698599</t>
-  </si>
-  <si>
-    <t>0697797-C</t>
-  </si>
-  <si>
-    <t>0697946-C</t>
-  </si>
-  <si>
-    <t>698748</t>
-  </si>
-  <si>
-    <t>0697948-C</t>
-  </si>
-  <si>
-    <t>698236</t>
-  </si>
-  <si>
-    <t>698235</t>
-  </si>
-  <si>
-    <t>698714</t>
-  </si>
-  <si>
-    <t>0698900-C</t>
-  </si>
-  <si>
-    <t>0698654-C</t>
-  </si>
-  <si>
-    <t>698918</t>
-  </si>
-  <si>
-    <t>0698913-C</t>
-  </si>
-  <si>
-    <t>0698916-C</t>
-  </si>
-  <si>
-    <t>4598-760-99</t>
-  </si>
-  <si>
-    <t>7555-617-70</t>
-  </si>
-  <si>
-    <t>B090-465-09</t>
-  </si>
-  <si>
-    <t>B090-B05-E3</t>
-  </si>
-  <si>
-    <t>B672-813-49</t>
-  </si>
-  <si>
-    <t>B090-B01-09</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>2022-04-15 00:00:00</t>
-  </si>
-  <si>
-    <t>2022-03-25 00:00:00</t>
-  </si>
-  <si>
-    <t>2022-04-20 00:00:00</t>
-  </si>
-  <si>
-    <t>2022-04-19 00:00:00</t>
-  </si>
-  <si>
-    <t>2022-04-22 00:00:00</t>
-  </si>
-  <si>
-    <t>2022-04-25 00:00:00</t>
+    <t>2022-04-05 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-04-06 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-04-07 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-04-08 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-04-12 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -611,13 +626,13 @@
         <v>16</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>570</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -626,7 +641,7 @@
         <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2">
         <v>54</v>
@@ -640,22 +655,22 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>137</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I3">
         <v>54</v>
@@ -669,22 +684,22 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>280</v>
+        <v>154</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G4" t="s">
         <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I4">
         <v>54</v>
@@ -698,22 +713,22 @@
         <v>17</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>802</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5">
         <v>54</v>
@@ -727,22 +742,22 @@
         <v>18</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>877</v>
+        <v>198</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I6">
         <v>54</v>
@@ -753,16 +768,16 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E7">
-        <v>891</v>
+        <v>4</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -771,7 +786,7 @@
         <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I7">
         <v>54</v>
@@ -782,19 +797,19 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E8">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G8" t="s">
         <v>19</v>
@@ -813,7 +828,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -853,25 +868,25 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>90</v>
+      </c>
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="E2">
-        <v>4745</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="I2">
         <v>55</v>
@@ -882,7 +897,7 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C3">
         <v>7</v>
@@ -891,16 +906,16 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H3" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="I3">
         <v>55</v>
@@ -911,22 +926,22 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>104</v>
+        <v>214</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H4" t="s">
         <v>23</v>
@@ -940,22 +955,22 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>5</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>669</v>
+        <v>508</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
         <v>22</v>
@@ -972,22 +987,22 @@
         <v>18</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D6">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>1223</v>
+      </c>
+      <c r="F6">
         <v>4</v>
       </c>
-      <c r="E6">
-        <v>1136</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I6">
         <v>55</v>
@@ -1001,22 +1016,22 @@
         <v>18</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E7">
-        <v>97</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I7">
         <v>55</v>
@@ -1027,25 +1042,25 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>296</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="I8">
         <v>55</v>
@@ -1056,25 +1071,25 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>857</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="H9" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="I9">
         <v>55</v>
@@ -1085,25 +1100,25 @@
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C10">
         <v>7</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H10" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="I10">
         <v>55</v>
@@ -1114,25 +1129,25 @@
         <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C11">
         <v>7</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="I11">
         <v>55</v>
@@ -1143,25 +1158,25 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C12">
         <v>7</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>239</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H12" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="I12">
         <v>55</v>
@@ -1172,25 +1187,25 @@
         <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C13">
         <v>7</v>
       </c>
       <c r="D13">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H13" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="I13">
         <v>55</v>
@@ -1201,25 +1216,25 @@
         <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C14">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D14">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>1502</v>
+        <v>2</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H14" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="I14">
         <v>55</v>
@@ -1230,25 +1245,25 @@
         <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C15">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D15">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>280</v>
+        <v>2</v>
       </c>
       <c r="F15">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H15" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="I15">
         <v>55</v>
@@ -1259,25 +1274,25 @@
         <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C16">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16">
-        <v>1670</v>
+        <v>62</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H16" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I16">
         <v>55</v>
@@ -1288,25 +1303,25 @@
         <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H17" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I17">
         <v>55</v>
@@ -1317,25 +1332,25 @@
         <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C18">
         <v>7</v>
       </c>
       <c r="D18">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>334</v>
+        <v>4</v>
       </c>
       <c r="F18">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H18" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I18">
         <v>55</v>
@@ -1346,7 +1361,7 @@
         <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C19">
         <v>7</v>
@@ -1355,16 +1370,16 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>688</v>
+        <v>133</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I19">
         <v>55</v>
@@ -1375,25 +1390,25 @@
         <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C20">
         <v>7</v>
       </c>
       <c r="D20">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H20" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I20">
         <v>55</v>
@@ -1404,7 +1419,7 @@
         <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C21">
         <v>7</v>
@@ -1413,16 +1428,16 @@
         <v>1</v>
       </c>
       <c r="E21">
-        <v>31</v>
+        <v>160</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H21" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I21">
         <v>55</v>
@@ -1433,25 +1448,25 @@
         <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C22">
         <v>7</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E22">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H22" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I22">
         <v>55</v>
@@ -1462,7 +1477,7 @@
         <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C23">
         <v>7</v>
@@ -1471,16 +1486,16 @@
         <v>1</v>
       </c>
       <c r="E23">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H23" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I23">
         <v>55</v>
@@ -1491,25 +1506,25 @@
         <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C24">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D24">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E24">
-        <v>528</v>
+        <v>514</v>
       </c>
       <c r="F24">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G24" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H24" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="I24">
         <v>55</v>
@@ -1520,25 +1535,25 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C25">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D25">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>388</v>
+        <v>17</v>
       </c>
       <c r="F25">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H25" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="I25">
         <v>55</v>
@@ -1549,25 +1564,25 @@
         <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C26">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H26" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I26">
         <v>55</v>
@@ -1578,25 +1593,25 @@
         <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C27">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D27">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>2726</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H27" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I27">
         <v>55</v>
@@ -1607,27 +1622,317 @@
         <v>51</v>
       </c>
       <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28">
+        <v>7</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>20</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>63</v>
+      </c>
+      <c r="H28" t="s">
+        <v>68</v>
+      </c>
+      <c r="I28">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>63</v>
+      </c>
+      <c r="H29" t="s">
+        <v>68</v>
+      </c>
+      <c r="I29">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30">
+        <v>7</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>223</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H30" t="s">
+        <v>69</v>
+      </c>
+      <c r="I30">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31">
+        <v>7</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31" t="s">
+        <v>63</v>
+      </c>
+      <c r="H31" t="s">
+        <v>69</v>
+      </c>
+      <c r="I31">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32">
+        <v>7</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>30</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
+        <v>63</v>
+      </c>
+      <c r="H32" t="s">
+        <v>69</v>
+      </c>
+      <c r="I32">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33">
+        <v>7</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33" t="s">
+        <v>63</v>
+      </c>
+      <c r="H33" t="s">
+        <v>69</v>
+      </c>
+      <c r="I33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
         <v>57</v>
       </c>
-      <c r="C28">
-        <v>9</v>
-      </c>
-      <c r="D28">
-        <v>15</v>
-      </c>
-      <c r="E28">
-        <v>133</v>
-      </c>
-      <c r="F28">
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>407</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
+        <v>63</v>
+      </c>
+      <c r="H34" t="s">
+        <v>69</v>
+      </c>
+      <c r="I34">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35">
+        <v>7</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>63</v>
+      </c>
+      <c r="H35" t="s">
+        <v>69</v>
+      </c>
+      <c r="I35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36">
+        <v>7</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>103</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
+        <v>63</v>
+      </c>
+      <c r="H36" t="s">
+        <v>69</v>
+      </c>
+      <c r="I36">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37">
+        <v>7</v>
+      </c>
+      <c r="D37">
+        <v>7</v>
+      </c>
+      <c r="E37">
+        <v>383</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37" t="s">
+        <v>63</v>
+      </c>
+      <c r="H37" t="s">
+        <v>69</v>
+      </c>
+      <c r="I37">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
         <v>2</v>
       </c>
-      <c r="G28" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" t="s">
-        <v>63</v>
-      </c>
-      <c r="I28">
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38" t="s">
+        <v>63</v>
+      </c>
+      <c r="H38" t="s">
+        <v>69</v>
+      </c>
+      <c r="I38">
         <v>55</v>
       </c>
     </row>
@@ -1638,7 +1943,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1681,13 +1986,13 @@
         <v>16</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>570</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1696,7 +2001,7 @@
         <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2">
         <v>54</v>
@@ -1710,22 +2015,22 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>137</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I3">
         <v>54</v>
@@ -1739,22 +2044,22 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>280</v>
+        <v>154</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G4" t="s">
         <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I4">
         <v>54</v>
@@ -1768,22 +2073,22 @@
         <v>17</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>802</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5">
         <v>54</v>
@@ -1797,22 +2102,22 @@
         <v>18</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>877</v>
+        <v>198</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I6">
         <v>54</v>
@@ -1823,16 +2128,16 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E7">
-        <v>891</v>
+        <v>4</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -1841,7 +2146,7 @@
         <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I7">
         <v>54</v>
@@ -1852,19 +2157,19 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E8">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G8" t="s">
         <v>19</v>
@@ -1881,25 +2186,25 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>90</v>
+      </c>
+      <c r="F9">
         <v>2</v>
       </c>
-      <c r="E9">
-        <v>4745</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
       <c r="G9" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H9" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="I9">
         <v>55</v>
@@ -1910,7 +2215,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C10">
         <v>7</v>
@@ -1919,16 +2224,16 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="I10">
         <v>55</v>
@@ -1939,22 +2244,22 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="C11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
-        <v>104</v>
+        <v>214</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H11" t="s">
         <v>23</v>
@@ -1968,22 +2273,22 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12">
         <v>5</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E12">
-        <v>669</v>
+        <v>508</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H12" t="s">
         <v>22</v>
@@ -2000,22 +2305,22 @@
         <v>18</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D13">
+        <v>14</v>
+      </c>
+      <c r="E13">
+        <v>1223</v>
+      </c>
+      <c r="F13">
         <v>4</v>
       </c>
-      <c r="E13">
-        <v>1136</v>
-      </c>
-      <c r="F13">
-        <v>5</v>
-      </c>
       <c r="G13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I13">
         <v>55</v>
@@ -2029,22 +2334,22 @@
         <v>18</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E14">
-        <v>97</v>
+        <v>9</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I14">
         <v>55</v>
@@ -2055,25 +2360,25 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>7</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>296</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="I15">
         <v>55</v>
@@ -2084,25 +2389,25 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <v>7</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>857</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="H16" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="I16">
         <v>55</v>
@@ -2113,25 +2418,25 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C17">
         <v>7</v>
       </c>
       <c r="D17">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H17" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="I17">
         <v>55</v>
@@ -2142,25 +2447,25 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C18">
         <v>7</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G18" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H18" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="I18">
         <v>55</v>
@@ -2171,25 +2476,25 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C19">
         <v>7</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>239</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H19" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="I19">
         <v>55</v>
@@ -2200,25 +2505,25 @@
         <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C20">
         <v>7</v>
       </c>
       <c r="D20">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="F20">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H20" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="I20">
         <v>55</v>
@@ -2229,25 +2534,25 @@
         <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C21">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D21">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>1502</v>
+        <v>2</v>
       </c>
       <c r="F21">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H21" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="I21">
         <v>55</v>
@@ -2258,25 +2563,25 @@
         <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D22">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>280</v>
+        <v>2</v>
       </c>
       <c r="F22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H22" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="I22">
         <v>55</v>
@@ -2287,25 +2592,25 @@
         <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C23">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23">
         <v>2</v>
       </c>
       <c r="E23">
-        <v>1670</v>
+        <v>62</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H23" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I23">
         <v>55</v>
@@ -2316,25 +2621,25 @@
         <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F24">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H24" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I24">
         <v>55</v>
@@ -2345,25 +2650,25 @@
         <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C25">
         <v>7</v>
       </c>
       <c r="D25">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>334</v>
+        <v>4</v>
       </c>
       <c r="F25">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H25" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I25">
         <v>55</v>
@@ -2374,7 +2679,7 @@
         <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C26">
         <v>7</v>
@@ -2383,16 +2688,16 @@
         <v>1</v>
       </c>
       <c r="E26">
-        <v>688</v>
+        <v>133</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H26" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I26">
         <v>55</v>
@@ -2403,25 +2708,25 @@
         <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C27">
         <v>7</v>
       </c>
       <c r="D27">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H27" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I27">
         <v>55</v>
@@ -2432,7 +2737,7 @@
         <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C28">
         <v>7</v>
@@ -2441,16 +2746,16 @@
         <v>1</v>
       </c>
       <c r="E28">
-        <v>31</v>
+        <v>160</v>
       </c>
       <c r="F28">
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H28" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I28">
         <v>55</v>
@@ -2461,25 +2766,25 @@
         <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C29">
         <v>7</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E29">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G29" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H29" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I29">
         <v>55</v>
@@ -2490,7 +2795,7 @@
         <v>46</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C30">
         <v>7</v>
@@ -2499,16 +2804,16 @@
         <v>1</v>
       </c>
       <c r="E30">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H30" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I30">
         <v>55</v>
@@ -2519,25 +2824,25 @@
         <v>47</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C31">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D31">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E31">
-        <v>528</v>
+        <v>514</v>
       </c>
       <c r="F31">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G31" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H31" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="I31">
         <v>55</v>
@@ -2548,25 +2853,25 @@
         <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C32">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D32">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E32">
-        <v>388</v>
+        <v>17</v>
       </c>
       <c r="F32">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H32" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="I32">
         <v>55</v>
@@ -2577,25 +2882,25 @@
         <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C33">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E33">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="F33">
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H33" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I33">
         <v>55</v>
@@ -2606,25 +2911,25 @@
         <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C34">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D34">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="E34">
-        <v>2726</v>
+        <v>0</v>
       </c>
       <c r="F34">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H34" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I34">
         <v>55</v>
@@ -2635,27 +2940,317 @@
         <v>51</v>
       </c>
       <c r="B35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35">
+        <v>7</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>20</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>63</v>
+      </c>
+      <c r="H35" t="s">
+        <v>68</v>
+      </c>
+      <c r="I35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36">
+        <v>7</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
+        <v>63</v>
+      </c>
+      <c r="H36" t="s">
+        <v>68</v>
+      </c>
+      <c r="I36">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37">
+        <v>7</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>223</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37" t="s">
+        <v>63</v>
+      </c>
+      <c r="H37" t="s">
+        <v>69</v>
+      </c>
+      <c r="I37">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38" t="s">
+        <v>63</v>
+      </c>
+      <c r="H38" t="s">
+        <v>69</v>
+      </c>
+      <c r="I38">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>30</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>63</v>
+      </c>
+      <c r="H39" t="s">
+        <v>69</v>
+      </c>
+      <c r="I39">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40">
+        <v>7</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40" t="s">
+        <v>63</v>
+      </c>
+      <c r="H40" t="s">
+        <v>69</v>
+      </c>
+      <c r="I40">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
         <v>57</v>
       </c>
-      <c r="C35">
-        <v>9</v>
-      </c>
-      <c r="D35">
-        <v>15</v>
-      </c>
-      <c r="E35">
-        <v>133</v>
-      </c>
-      <c r="F35">
+      <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41">
+        <v>7</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>407</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41" t="s">
+        <v>63</v>
+      </c>
+      <c r="H41" t="s">
+        <v>69</v>
+      </c>
+      <c r="I41">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42">
+        <v>7</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42" t="s">
+        <v>63</v>
+      </c>
+      <c r="H42" t="s">
+        <v>69</v>
+      </c>
+      <c r="I42">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43">
+        <v>7</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>103</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43" t="s">
+        <v>63</v>
+      </c>
+      <c r="H43" t="s">
+        <v>69</v>
+      </c>
+      <c r="I43">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44">
+        <v>7</v>
+      </c>
+      <c r="D44">
+        <v>7</v>
+      </c>
+      <c r="E44">
+        <v>383</v>
+      </c>
+      <c r="F44">
+        <v>3</v>
+      </c>
+      <c r="G44" t="s">
+        <v>63</v>
+      </c>
+      <c r="H44" t="s">
+        <v>69</v>
+      </c>
+      <c r="I44">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45">
+        <v>7</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
         <v>2</v>
       </c>
-      <c r="G35" t="s">
-        <v>20</v>
-      </c>
-      <c r="H35" t="s">
-        <v>63</v>
-      </c>
-      <c r="I35">
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45" t="s">
+        <v>63</v>
+      </c>
+      <c r="H45" t="s">
+        <v>69</v>
+      </c>
+      <c r="I45">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
na schedule balancing across the two machines
</commit_message>
<xml_diff>
--- a/schedules.xlsx
+++ b/schedules.xlsx
@@ -45,76 +45,76 @@
     <t>Scheduled Machine</t>
   </si>
   <si>
+    <t>697124</t>
+  </si>
+  <si>
+    <t>697125</t>
+  </si>
+  <si>
     <t>697612</t>
   </si>
   <si>
-    <t>697124</t>
-  </si>
-  <si>
-    <t>697125</t>
+    <t>0697006-C</t>
   </si>
   <si>
     <t>0696823-C</t>
   </si>
   <si>
+    <t>0697925-C</t>
+  </si>
+  <si>
+    <t>0697923-C</t>
+  </si>
+  <si>
+    <t>0697922-C</t>
+  </si>
+  <si>
+    <t>697921</t>
+  </si>
+  <si>
     <t>697927</t>
   </si>
   <si>
     <t>0696949-C</t>
   </si>
   <si>
+    <t>B670-813-49</t>
+  </si>
+  <si>
+    <t>B672-813-49</t>
+  </si>
+  <si>
+    <t>C193-602-70</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>2022-03-25 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-03-22 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-03-29 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-03-30 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>0696893-C</t>
+  </si>
+  <si>
+    <t>697005</t>
+  </si>
+  <si>
+    <t>0697360-C</t>
+  </si>
+  <si>
     <t>0696782-C</t>
-  </si>
-  <si>
-    <t>B670-813-49</t>
-  </si>
-  <si>
-    <t>B672-813-49</t>
-  </si>
-  <si>
-    <t>C193-602-70</t>
-  </si>
-  <si>
-    <t>na</t>
-  </si>
-  <si>
-    <t>2022-03-22 00:00:00</t>
-  </si>
-  <si>
-    <t>2022-03-25 00:00:00</t>
-  </si>
-  <si>
-    <t>2022-03-29 00:00:00</t>
-  </si>
-  <si>
-    <t>2022-03-30 00:00:00</t>
-  </si>
-  <si>
-    <t>2022-04-01 00:00:00</t>
-  </si>
-  <si>
-    <t>0696893-C</t>
-  </si>
-  <si>
-    <t>697005</t>
-  </si>
-  <si>
-    <t>0697360-C</t>
-  </si>
-  <si>
-    <t>0697006-C</t>
-  </si>
-  <si>
-    <t>0697925-C</t>
-  </si>
-  <si>
-    <t>0697923-C</t>
-  </si>
-  <si>
-    <t>0697922-C</t>
-  </si>
-  <si>
-    <t>697921</t>
   </si>
   <si>
     <t>696720</t>
@@ -583,7 +583,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -623,25 +623,25 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>570</v>
+        <v>137</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="I2">
         <v>54</v>
@@ -652,7 +652,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -661,16 +661,16 @@
         <v>5</v>
       </c>
       <c r="E3">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I3">
         <v>54</v>
@@ -681,25 +681,25 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>5</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4">
-        <v>154</v>
+        <v>570</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I4">
         <v>54</v>
@@ -710,7 +710,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -719,16 +719,16 @@
         <v>5</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>508</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I5">
         <v>54</v>
@@ -739,25 +739,25 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I6">
         <v>54</v>
@@ -768,25 +768,25 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E7">
+        <v>1223</v>
+      </c>
+      <c r="F7">
         <v>4</v>
       </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I7">
         <v>54</v>
@@ -797,27 +797,143 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>9</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="E9">
+        <v>296</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="C8">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>857</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>198</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
         <v>5</v>
       </c>
-      <c r="D8">
-        <v>12</v>
-      </c>
-      <c r="E8">
-        <v>166</v>
-      </c>
-      <c r="F8">
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
         <v>2</v>
       </c>
-      <c r="G8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8">
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12">
         <v>54</v>
       </c>
     </row>
@@ -828,7 +944,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -865,7 +981,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>62</v>
@@ -886,7 +1002,7 @@
         <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I2">
         <v>55</v>
@@ -894,7 +1010,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>62</v>
@@ -915,7 +1031,7 @@
         <v>63</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I3">
         <v>55</v>
@@ -923,7 +1039,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>62</v>
@@ -944,7 +1060,7 @@
         <v>63</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I4">
         <v>55</v>
@@ -952,28 +1068,28 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>5</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E5">
-        <v>508</v>
+        <v>166</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I5">
         <v>55</v>
@@ -981,28 +1097,28 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C6">
         <v>7</v>
       </c>
       <c r="D6">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>1223</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="I6">
         <v>55</v>
@@ -1010,28 +1126,28 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C7">
         <v>7</v>
       </c>
       <c r="D7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7">
-        <v>9</v>
+        <v>113</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="H7" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="I7">
         <v>55</v>
@@ -1039,28 +1155,28 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>296</v>
+        <v>239</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="H8" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="I8">
         <v>55</v>
@@ -1068,28 +1184,28 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>857</v>
+        <v>8</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="H9" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="I9">
         <v>55</v>
@@ -1097,7 +1213,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>62</v>
@@ -1109,7 +1225,7 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1118,7 +1234,7 @@
         <v>63</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="I10">
         <v>55</v>
@@ -1126,7 +1242,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>62</v>
@@ -1135,19 +1251,19 @@
         <v>7</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>113</v>
+        <v>2</v>
       </c>
       <c r="F11">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G11" t="s">
         <v>63</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I11">
         <v>55</v>
@@ -1155,7 +1271,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
         <v>62</v>
@@ -1167,7 +1283,7 @@
         <v>2</v>
       </c>
       <c r="E12">
-        <v>239</v>
+        <v>62</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1176,7 +1292,7 @@
         <v>63</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I12">
         <v>55</v>
@@ -1184,7 +1300,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
         <v>62</v>
@@ -1196,7 +1312,7 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1205,7 +1321,7 @@
         <v>63</v>
       </c>
       <c r="H13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I13">
         <v>55</v>
@@ -1213,7 +1329,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
         <v>62</v>
@@ -1225,7 +1341,7 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1242,7 +1358,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
         <v>62</v>
@@ -1254,7 +1370,7 @@
         <v>1</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>133</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1271,7 +1387,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
         <v>62</v>
@@ -1280,10 +1396,10 @@
         <v>7</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1300,7 +1416,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
         <v>62</v>
@@ -1312,7 +1428,7 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>160</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1321,7 +1437,7 @@
         <v>63</v>
       </c>
       <c r="H17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I17">
         <v>55</v>
@@ -1329,7 +1445,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
         <v>62</v>
@@ -1338,19 +1454,19 @@
         <v>7</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G18" t="s">
         <v>63</v>
       </c>
       <c r="H18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I18">
         <v>55</v>
@@ -1358,7 +1474,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
         <v>62</v>
@@ -1370,7 +1486,7 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>133</v>
+        <v>2</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1379,7 +1495,7 @@
         <v>63</v>
       </c>
       <c r="H19" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I19">
         <v>55</v>
@@ -1387,7 +1503,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
         <v>62</v>
@@ -1396,19 +1512,19 @@
         <v>7</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>514</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G20" t="s">
         <v>63</v>
       </c>
       <c r="H20" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I20">
         <v>55</v>
@@ -1416,7 +1532,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
         <v>62</v>
@@ -1428,7 +1544,7 @@
         <v>1</v>
       </c>
       <c r="E21">
-        <v>160</v>
+        <v>17</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1437,7 +1553,7 @@
         <v>63</v>
       </c>
       <c r="H21" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I21">
         <v>55</v>
@@ -1445,7 +1561,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
         <v>62</v>
@@ -1457,16 +1573,16 @@
         <v>3</v>
       </c>
       <c r="E22">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="F22">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G22" t="s">
         <v>63</v>
       </c>
       <c r="H22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I22">
         <v>55</v>
@@ -1474,7 +1590,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
         <v>62</v>
@@ -1486,7 +1602,7 @@
         <v>1</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1503,7 +1619,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
         <v>62</v>
@@ -1512,13 +1628,13 @@
         <v>7</v>
       </c>
       <c r="D24">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>514</v>
+        <v>20</v>
       </c>
       <c r="F24">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G24" t="s">
         <v>63</v>
@@ -1532,7 +1648,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
         <v>62</v>
@@ -1544,7 +1660,7 @@
         <v>1</v>
       </c>
       <c r="E25">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1561,7 +1677,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
         <v>62</v>
@@ -1570,10 +1686,10 @@
         <v>7</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>64</v>
+        <v>223</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1582,7 +1698,7 @@
         <v>63</v>
       </c>
       <c r="H26" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I26">
         <v>55</v>
@@ -1590,7 +1706,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
         <v>62</v>
@@ -1602,7 +1718,7 @@
         <v>1</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1611,7 +1727,7 @@
         <v>63</v>
       </c>
       <c r="H27" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I27">
         <v>55</v>
@@ -1619,7 +1735,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
         <v>62</v>
@@ -1631,7 +1747,7 @@
         <v>1</v>
       </c>
       <c r="E28">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -1640,7 +1756,7 @@
         <v>63</v>
       </c>
       <c r="H28" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I28">
         <v>55</v>
@@ -1648,7 +1764,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
         <v>62</v>
@@ -1660,7 +1776,7 @@
         <v>1</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -1669,7 +1785,7 @@
         <v>63</v>
       </c>
       <c r="H29" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I29">
         <v>55</v>
@@ -1677,7 +1793,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
         <v>62</v>
@@ -1689,7 +1805,7 @@
         <v>1</v>
       </c>
       <c r="E30">
-        <v>223</v>
+        <v>407</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1706,7 +1822,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
         <v>62</v>
@@ -1735,7 +1851,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
         <v>62</v>
@@ -1747,7 +1863,7 @@
         <v>1</v>
       </c>
       <c r="E32">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1764,7 +1880,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
         <v>62</v>
@@ -1773,13 +1889,13 @@
         <v>7</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E33">
+        <v>383</v>
+      </c>
+      <c r="F33">
         <v>3</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
       </c>
       <c r="G33" t="s">
         <v>63</v>
@@ -1793,7 +1909,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B34" t="s">
         <v>62</v>
@@ -1805,7 +1921,7 @@
         <v>1</v>
       </c>
       <c r="E34">
-        <v>407</v>
+        <v>2</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1817,122 +1933,6 @@
         <v>69</v>
       </c>
       <c r="I34">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35">
-        <v>7</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>3</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35" t="s">
-        <v>63</v>
-      </c>
-      <c r="H35" t="s">
-        <v>69</v>
-      </c>
-      <c r="I35">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" t="s">
-        <v>62</v>
-      </c>
-      <c r="C36">
-        <v>7</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36">
-        <v>103</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36" t="s">
-        <v>63</v>
-      </c>
-      <c r="H36" t="s">
-        <v>69</v>
-      </c>
-      <c r="I36">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" t="s">
-        <v>60</v>
-      </c>
-      <c r="B37" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37">
-        <v>7</v>
-      </c>
-      <c r="D37">
-        <v>7</v>
-      </c>
-      <c r="E37">
-        <v>383</v>
-      </c>
-      <c r="F37">
-        <v>3</v>
-      </c>
-      <c r="G37" t="s">
-        <v>63</v>
-      </c>
-      <c r="H37" t="s">
-        <v>69</v>
-      </c>
-      <c r="I37">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" t="s">
-        <v>61</v>
-      </c>
-      <c r="B38" t="s">
-        <v>62</v>
-      </c>
-      <c r="C38">
-        <v>7</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>2</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38" t="s">
-        <v>63</v>
-      </c>
-      <c r="H38" t="s">
-        <v>69</v>
-      </c>
-      <c r="I38">
         <v>55</v>
       </c>
     </row>
@@ -1983,25 +1983,25 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>570</v>
+        <v>137</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="I2">
         <v>54</v>
@@ -2012,7 +2012,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -2021,16 +2021,16 @@
         <v>5</v>
       </c>
       <c r="E3">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I3">
         <v>54</v>
@@ -2041,25 +2041,25 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>5</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4">
-        <v>154</v>
+        <v>570</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I4">
         <v>54</v>
@@ -2070,7 +2070,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -2079,16 +2079,16 @@
         <v>5</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>508</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I5">
         <v>54</v>
@@ -2099,25 +2099,25 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I6">
         <v>54</v>
@@ -2128,25 +2128,25 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E7">
+        <v>1223</v>
+      </c>
+      <c r="F7">
         <v>4</v>
       </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I7">
         <v>54</v>
@@ -2157,25 +2157,25 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D8">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E8">
-        <v>166</v>
+        <v>9</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I8">
         <v>54</v>
@@ -2183,97 +2183,97 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E9">
-        <v>90</v>
+        <v>296</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I9">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>7</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>857</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="H10" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I10">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>198</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11">
-        <v>7</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>214</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
-      <c r="G11" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" t="s">
-        <v>23</v>
-      </c>
       <c r="I11">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -2282,19 +2282,19 @@
         <v>5</v>
       </c>
       <c r="E12">
-        <v>508</v>
+        <v>4</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H12" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I12">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -2302,25 +2302,25 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C13">
         <v>7</v>
       </c>
       <c r="D13">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>1223</v>
+        <v>90</v>
       </c>
       <c r="F13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="H13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I13">
         <v>55</v>
@@ -2331,25 +2331,25 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C14">
         <v>7</v>
       </c>
       <c r="D14">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="H14" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I14">
         <v>55</v>
@@ -2360,25 +2360,25 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C15">
         <v>7</v>
       </c>
       <c r="D15">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>296</v>
+        <v>214</v>
       </c>
       <c r="F15">
         <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="H15" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I15">
         <v>55</v>
@@ -2389,25 +2389,25 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C16">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E16">
-        <v>857</v>
+        <v>166</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H16" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="I16">
         <v>55</v>
@@ -2436,7 +2436,7 @@
         <v>63</v>
       </c>
       <c r="H17" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I17">
         <v>55</v>

</xml_diff>